<commit_message>
~ Resultados actualizados +1
</commit_message>
<xml_diff>
--- a/resultados tripla.xlsx
+++ b/resultados tripla.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SIGN</t>
   </si>
@@ -51,7 +51,10 @@
     <t>MAQUINA 3G</t>
   </si>
   <si>
-    <t>ANTÒNIO</t>
+    <t>BEATRIZ</t>
+  </si>
+  <si>
+    <t>ANTÓNIO</t>
   </si>
 </sst>
 </file>
@@ -386,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O245"/>
+  <dimension ref="A1:P245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N245" sqref="N245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,10 +404,11 @@
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="16" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,10 +431,13 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -469,7 +476,7 @@
       </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1</v>
       </c>
@@ -503,12 +510,12 @@
         <v>2</v>
       </c>
       <c r="L3" t="b">
-        <f t="shared" ref="L3:N66" si="5">(-1*(K3-2))=A3</f>
+        <f t="shared" ref="L3:L66" si="5">(-1*(K3-2))=A3</f>
         <v>0</v>
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>1</v>
       </c>
@@ -547,7 +554,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -586,7 +593,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>1</v>
       </c>
@@ -625,7 +632,7 @@
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>1</v>
       </c>
@@ -668,8 +675,11 @@
       <c r="N7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>-1</v>
       </c>
@@ -712,8 +722,11 @@
       <c r="N8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>1</v>
       </c>
@@ -756,8 +769,11 @@
       <c r="N9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -800,8 +816,11 @@
       <c r="N10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>1</v>
       </c>
@@ -839,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>-1</v>
       </c>
@@ -878,7 +897,7 @@
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>1</v>
       </c>
@@ -921,8 +940,11 @@
       <c r="N13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>0</v>
       </c>
@@ -961,7 +983,7 @@
       </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1004,8 +1026,11 @@
       <c r="N15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1044,7 +1069,7 @@
       </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1083,7 +1108,7 @@
       </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>-1</v>
       </c>
@@ -1122,7 +1147,7 @@
       </c>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1165,8 +1190,11 @@
       <c r="N19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="P19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1205,7 +1233,7 @@
       </c>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>-1</v>
       </c>
@@ -1244,7 +1272,7 @@
       </c>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:16">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1283,7 +1311,7 @@
       </c>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:16">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1322,7 +1350,7 @@
       </c>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:16">
       <c r="A24">
         <v>-1</v>
       </c>
@@ -1365,8 +1393,11 @@
       <c r="N24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1405,7 +1436,7 @@
       </c>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:16">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1448,8 +1479,11 @@
       <c r="N26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1492,8 +1526,11 @@
       <c r="N27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="P27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28">
         <v>-1</v>
       </c>
@@ -1532,7 +1569,7 @@
       </c>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:16">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1571,7 +1608,7 @@
       </c>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:16">
       <c r="A30">
         <v>-1</v>
       </c>
@@ -1610,7 +1647,7 @@
       </c>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:16">
       <c r="A31">
         <v>-1</v>
       </c>
@@ -1653,8 +1690,11 @@
       <c r="N31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="P31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32">
         <v>-1</v>
       </c>
@@ -1693,7 +1733,7 @@
       </c>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:16">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1732,7 +1772,7 @@
       </c>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:16">
       <c r="A34">
         <v>-1</v>
       </c>
@@ -1771,7 +1811,7 @@
       </c>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:16">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1810,7 +1850,7 @@
       </c>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:16">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1849,7 +1889,7 @@
       </c>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:16">
       <c r="A37">
         <v>0</v>
       </c>
@@ -1892,8 +1932,11 @@
       <c r="N37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="P37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38">
         <v>0</v>
       </c>
@@ -1936,8 +1979,11 @@
       <c r="N38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="P38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39">
         <v>-1</v>
       </c>
@@ -1980,8 +2026,11 @@
       <c r="N39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="P39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2020,7 +2069,7 @@
       </c>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:16">
       <c r="A41">
         <v>0</v>
       </c>
@@ -2059,7 +2108,7 @@
       </c>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:16">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2102,8 +2151,11 @@
       <c r="N42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="P42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43">
         <v>0</v>
       </c>
@@ -2142,7 +2194,7 @@
       </c>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:16">
       <c r="A44">
         <v>0</v>
       </c>
@@ -2185,8 +2237,11 @@
       <c r="N44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="P44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45">
         <v>-1</v>
       </c>
@@ -2225,7 +2280,7 @@
       </c>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:16">
       <c r="A46">
         <v>-1</v>
       </c>
@@ -2264,7 +2319,7 @@
       </c>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:16">
       <c r="A47">
         <v>-1</v>
       </c>
@@ -2303,7 +2358,7 @@
       </c>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:16">
       <c r="A48">
         <v>-1</v>
       </c>
@@ -2346,8 +2401,11 @@
       <c r="N48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="P48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49">
         <v>0</v>
       </c>
@@ -2386,7 +2444,7 @@
       </c>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:16">
       <c r="A50">
         <v>-1</v>
       </c>
@@ -2425,7 +2483,7 @@
       </c>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:16">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2464,7 +2522,7 @@
       </c>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2507,8 +2565,11 @@
       <c r="N52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="P52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53">
         <v>-1</v>
       </c>
@@ -2551,8 +2612,11 @@
       <c r="N53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="P53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54">
         <v>-1</v>
       </c>
@@ -2595,8 +2659,11 @@
       <c r="N54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="P54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2635,7 +2702,7 @@
       </c>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:16">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2674,7 +2741,7 @@
       </c>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:16">
       <c r="A57">
         <v>1</v>
       </c>
@@ -2713,7 +2780,7 @@
       </c>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:16">
       <c r="A58">
         <v>-1</v>
       </c>
@@ -2752,7 +2819,7 @@
       </c>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:16">
       <c r="A59">
         <v>1</v>
       </c>
@@ -2791,7 +2858,7 @@
       </c>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:16">
       <c r="A60">
         <v>-1</v>
       </c>
@@ -2830,7 +2897,7 @@
       </c>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:16">
       <c r="A61">
         <v>0</v>
       </c>
@@ -2869,7 +2936,7 @@
       </c>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:16">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2912,8 +2979,11 @@
       <c r="N62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="P62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63">
         <v>-1</v>
       </c>
@@ -2952,7 +3022,7 @@
       </c>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:16">
       <c r="A64">
         <v>1</v>
       </c>
@@ -2995,8 +3065,11 @@
       <c r="N64" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="P64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65">
         <v>-1</v>
       </c>
@@ -3035,7 +3108,7 @@
       </c>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:16">
       <c r="A66">
         <v>-1</v>
       </c>
@@ -3078,8 +3151,11 @@
       <c r="N66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="P66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67">
         <v>0</v>
       </c>
@@ -3113,7 +3189,7 @@
         <v>3</v>
       </c>
       <c r="L67" t="b">
-        <f t="shared" ref="L67:N130" si="11">(-1*(K67-2))=A67</f>
+        <f t="shared" ref="L67:L130" si="11">(-1*(K67-2))=A67</f>
         <v>0</v>
       </c>
       <c r="M67" s="1" t="b">
@@ -3122,8 +3198,11 @@
       <c r="N67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="P67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68">
         <v>1</v>
       </c>
@@ -3166,8 +3245,11 @@
       <c r="N68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="P68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69">
         <v>0</v>
       </c>
@@ -3206,7 +3288,7 @@
       </c>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:16">
       <c r="A70">
         <v>-1</v>
       </c>
@@ -3245,7 +3327,7 @@
       </c>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:16">
       <c r="A71">
         <v>1</v>
       </c>
@@ -3284,7 +3366,7 @@
       </c>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:16">
       <c r="A72">
         <v>0</v>
       </c>
@@ -3323,7 +3405,7 @@
       </c>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:16">
       <c r="A73">
         <v>-1</v>
       </c>
@@ -3362,7 +3444,7 @@
       </c>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:16">
       <c r="A74">
         <v>1</v>
       </c>
@@ -3405,8 +3487,11 @@
       <c r="N74" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="P74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75">
         <v>0</v>
       </c>
@@ -3449,8 +3534,11 @@
       <c r="N75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="P75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76">
         <v>-1</v>
       </c>
@@ -3493,8 +3581,11 @@
       <c r="N76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:14">
+      <c r="P76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77">
         <v>1</v>
       </c>
@@ -3533,7 +3624,7 @@
       </c>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:16">
       <c r="A78">
         <v>1</v>
       </c>
@@ -3572,7 +3663,7 @@
       </c>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:16">
       <c r="A79">
         <v>-1</v>
       </c>
@@ -3611,7 +3702,7 @@
       </c>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:16">
       <c r="A80">
         <v>1</v>
       </c>
@@ -3650,7 +3741,7 @@
       </c>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:16">
       <c r="A81">
         <v>-1</v>
       </c>
@@ -3689,7 +3780,7 @@
       </c>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:16">
       <c r="A82">
         <v>1</v>
       </c>
@@ -3728,7 +3819,7 @@
       </c>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:16">
       <c r="A83">
         <v>1</v>
       </c>
@@ -3771,8 +3862,11 @@
       <c r="N83" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="P83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84">
         <v>-1</v>
       </c>
@@ -3811,7 +3905,7 @@
       </c>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:16">
       <c r="A85">
         <v>0</v>
       </c>
@@ -3850,7 +3944,7 @@
       </c>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:16">
       <c r="A86">
         <v>0</v>
       </c>
@@ -3889,7 +3983,7 @@
       </c>
       <c r="M86" s="1"/>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:16">
       <c r="A87">
         <v>-1</v>
       </c>
@@ -3932,8 +4026,11 @@
       <c r="N87" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="P87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88">
         <v>1</v>
       </c>
@@ -3976,8 +4073,11 @@
       <c r="N88" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="P88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89">
         <v>-1</v>
       </c>
@@ -4016,7 +4116,7 @@
       </c>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:16">
       <c r="A90">
         <v>0</v>
       </c>
@@ -4059,8 +4159,11 @@
       <c r="N90" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="P90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91">
         <v>0</v>
       </c>
@@ -4099,7 +4202,7 @@
       </c>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:16">
       <c r="A92">
         <v>-1</v>
       </c>
@@ -4138,7 +4241,7 @@
       </c>
       <c r="M92" s="1"/>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:16">
       <c r="A93">
         <v>1</v>
       </c>
@@ -4181,8 +4284,11 @@
       <c r="N93" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:14">
+      <c r="P93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94">
         <v>-1</v>
       </c>
@@ -4225,8 +4331,11 @@
       <c r="N94" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:14">
+      <c r="P94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="A95">
         <v>0</v>
       </c>
@@ -4265,7 +4374,7 @@
       </c>
       <c r="M95" s="1"/>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:16">
       <c r="A96">
         <v>-1</v>
       </c>
@@ -4304,7 +4413,7 @@
       </c>
       <c r="M96" s="1"/>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:16">
       <c r="A97">
         <v>1</v>
       </c>
@@ -4343,7 +4452,7 @@
       </c>
       <c r="M97" s="1"/>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:16">
       <c r="A98">
         <v>0</v>
       </c>
@@ -4382,7 +4491,7 @@
       </c>
       <c r="M98" s="1"/>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:16">
       <c r="A99">
         <v>1</v>
       </c>
@@ -4421,7 +4530,7 @@
       </c>
       <c r="M99" s="1"/>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:16">
       <c r="A100">
         <v>1</v>
       </c>
@@ -4464,8 +4573,11 @@
       <c r="N100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:14">
+      <c r="P100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16">
       <c r="A101">
         <v>-1</v>
       </c>
@@ -4504,7 +4616,7 @@
       </c>
       <c r="M101" s="1"/>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:16">
       <c r="A102">
         <v>-1</v>
       </c>
@@ -4547,8 +4659,11 @@
       <c r="N102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:14">
+      <c r="P102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16">
       <c r="A103">
         <v>-1</v>
       </c>
@@ -4591,8 +4706,11 @@
       <c r="N103" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:14">
+      <c r="P103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16">
       <c r="A104">
         <v>1</v>
       </c>
@@ -4631,7 +4749,7 @@
       </c>
       <c r="M104" s="1"/>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:16">
       <c r="A105">
         <v>1</v>
       </c>
@@ -4670,7 +4788,7 @@
       </c>
       <c r="M105" s="1"/>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:16">
       <c r="A106">
         <v>0</v>
       </c>
@@ -4709,7 +4827,7 @@
       </c>
       <c r="M106" s="1"/>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:16">
       <c r="A107">
         <v>1</v>
       </c>
@@ -4752,8 +4870,11 @@
       <c r="N107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:14">
+      <c r="P107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16">
       <c r="A108">
         <v>-1</v>
       </c>
@@ -4796,8 +4917,11 @@
       <c r="N108" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:14">
+      <c r="P108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16">
       <c r="A109">
         <v>1</v>
       </c>
@@ -4836,7 +4960,7 @@
       </c>
       <c r="M109" s="1"/>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:16">
       <c r="A110">
         <v>0</v>
       </c>
@@ -4875,7 +4999,7 @@
       </c>
       <c r="M110" s="1"/>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:16">
       <c r="A111">
         <v>0</v>
       </c>
@@ -4918,8 +5042,11 @@
       <c r="N111" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:14">
+      <c r="P111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16">
       <c r="A112">
         <v>0</v>
       </c>
@@ -4956,14 +5083,9 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M112" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="N112" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14">
+      <c r="M112" s="1"/>
+    </row>
+    <row r="113" spans="1:16">
       <c r="A113">
         <v>-1</v>
       </c>
@@ -5002,7 +5124,7 @@
       </c>
       <c r="M113" s="1"/>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:16">
       <c r="A114">
         <v>1</v>
       </c>
@@ -5041,7 +5163,7 @@
       </c>
       <c r="M114" s="1"/>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:16">
       <c r="A115">
         <v>0</v>
       </c>
@@ -5078,9 +5200,17 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M115" s="1"/>
-    </row>
-    <row r="116" spans="1:14">
+      <c r="M115" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N115" t="b">
+        <v>0</v>
+      </c>
+      <c r="P115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
       <c r="A116">
         <v>0</v>
       </c>
@@ -5119,7 +5249,7 @@
       </c>
       <c r="M116" s="1"/>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:16">
       <c r="A117">
         <v>1</v>
       </c>
@@ -5158,7 +5288,7 @@
       </c>
       <c r="M117" s="1"/>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:16">
       <c r="A118">
         <v>1</v>
       </c>
@@ -5197,7 +5327,7 @@
       </c>
       <c r="M118" s="1"/>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:16">
       <c r="A119">
         <v>1</v>
       </c>
@@ -5240,8 +5370,11 @@
       <c r="N119" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:14">
+      <c r="P119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16">
       <c r="A120">
         <v>1</v>
       </c>
@@ -5280,7 +5413,7 @@
       </c>
       <c r="M120" s="1"/>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:16">
       <c r="A121">
         <v>1</v>
       </c>
@@ -5319,7 +5452,7 @@
       </c>
       <c r="M121" s="1"/>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:16">
       <c r="A122">
         <v>-1</v>
       </c>
@@ -5358,7 +5491,7 @@
       </c>
       <c r="M122" s="1"/>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:16">
       <c r="A123">
         <v>-1</v>
       </c>
@@ -5401,8 +5534,11 @@
       <c r="N123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:14">
+      <c r="P123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16">
       <c r="A124">
         <v>1</v>
       </c>
@@ -5441,7 +5577,7 @@
       </c>
       <c r="M124" s="1"/>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:16">
       <c r="A125">
         <v>1</v>
       </c>
@@ -5484,8 +5620,11 @@
       <c r="N125" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:14">
+      <c r="P125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16">
       <c r="A126">
         <v>1</v>
       </c>
@@ -5528,8 +5667,11 @@
       <c r="N126" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:14">
+      <c r="P126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16">
       <c r="A127">
         <v>1</v>
       </c>
@@ -5568,7 +5710,7 @@
       </c>
       <c r="M127" s="1"/>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:16">
       <c r="A128">
         <v>0</v>
       </c>
@@ -5607,7 +5749,7 @@
       </c>
       <c r="M128" s="1"/>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:16">
       <c r="A129">
         <v>0</v>
       </c>
@@ -5646,7 +5788,7 @@
       </c>
       <c r="M129" s="1"/>
     </row>
-    <row r="130" spans="1:14">
+    <row r="130" spans="1:16">
       <c r="A130">
         <v>0</v>
       </c>
@@ -5685,7 +5827,7 @@
       </c>
       <c r="M130" s="1"/>
     </row>
-    <row r="131" spans="1:14">
+    <row r="131" spans="1:16">
       <c r="A131">
         <v>0</v>
       </c>
@@ -5719,7 +5861,7 @@
         <v>3</v>
       </c>
       <c r="L131" t="b">
-        <f t="shared" ref="L131:N194" si="17">(-1*(K131-2))=A131</f>
+        <f t="shared" ref="L131:L194" si="17">(-1*(K131-2))=A131</f>
         <v>0</v>
       </c>
       <c r="M131" s="1" t="b">
@@ -5728,8 +5870,11 @@
       <c r="N131" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:14">
+      <c r="P131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16">
       <c r="A132">
         <v>1</v>
       </c>
@@ -5772,8 +5917,11 @@
       <c r="N132" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:14">
+      <c r="P132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16">
       <c r="A133">
         <v>1</v>
       </c>
@@ -5812,7 +5960,7 @@
       </c>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:16">
       <c r="A134">
         <v>1</v>
       </c>
@@ -5851,7 +5999,7 @@
       </c>
       <c r="M134" s="1"/>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:16">
       <c r="A135">
         <v>0</v>
       </c>
@@ -5894,8 +6042,11 @@
       <c r="N135" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:14">
+      <c r="P135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16">
       <c r="A136">
         <v>-1</v>
       </c>
@@ -5934,7 +6085,7 @@
       </c>
       <c r="M136" s="1"/>
     </row>
-    <row r="137" spans="1:14">
+    <row r="137" spans="1:16">
       <c r="A137">
         <v>1</v>
       </c>
@@ -5973,7 +6124,7 @@
       </c>
       <c r="M137" s="1"/>
     </row>
-    <row r="138" spans="1:14">
+    <row r="138" spans="1:16">
       <c r="A138">
         <v>1</v>
       </c>
@@ -6012,7 +6163,7 @@
       </c>
       <c r="M138" s="1"/>
     </row>
-    <row r="139" spans="1:14">
+    <row r="139" spans="1:16">
       <c r="A139">
         <v>1</v>
       </c>
@@ -6051,7 +6202,7 @@
       </c>
       <c r="M139" s="1"/>
     </row>
-    <row r="140" spans="1:14">
+    <row r="140" spans="1:16">
       <c r="A140">
         <v>0</v>
       </c>
@@ -6090,7 +6241,7 @@
       </c>
       <c r="M140" s="1"/>
     </row>
-    <row r="141" spans="1:14">
+    <row r="141" spans="1:16">
       <c r="A141">
         <v>1</v>
       </c>
@@ -6133,8 +6284,11 @@
       <c r="N141" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:14">
+      <c r="P141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16">
       <c r="A142">
         <v>0</v>
       </c>
@@ -6173,7 +6327,7 @@
       </c>
       <c r="M142" s="1"/>
     </row>
-    <row r="143" spans="1:14">
+    <row r="143" spans="1:16">
       <c r="A143">
         <v>1</v>
       </c>
@@ -6212,7 +6366,7 @@
       </c>
       <c r="M143" s="1"/>
     </row>
-    <row r="144" spans="1:14">
+    <row r="144" spans="1:16">
       <c r="A144">
         <v>-1</v>
       </c>
@@ -6251,7 +6405,7 @@
       </c>
       <c r="M144" s="1"/>
     </row>
-    <row r="145" spans="1:14">
+    <row r="145" spans="1:16">
       <c r="A145">
         <v>1</v>
       </c>
@@ -6294,8 +6448,11 @@
       <c r="N145" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:14">
+      <c r="P145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16">
       <c r="A146">
         <v>0</v>
       </c>
@@ -6334,7 +6491,7 @@
       </c>
       <c r="M146" s="1"/>
     </row>
-    <row r="147" spans="1:14">
+    <row r="147" spans="1:16">
       <c r="A147">
         <v>1</v>
       </c>
@@ -6377,8 +6534,11 @@
       <c r="N147" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:14">
+      <c r="P147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16">
       <c r="A148">
         <v>0</v>
       </c>
@@ -6417,7 +6577,7 @@
       </c>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="1:14">
+    <row r="149" spans="1:16">
       <c r="A149">
         <v>-1</v>
       </c>
@@ -6460,8 +6620,11 @@
       <c r="N149" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:14">
+      <c r="P149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16">
       <c r="A150">
         <v>1</v>
       </c>
@@ -6500,7 +6663,7 @@
       </c>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:16">
       <c r="A151">
         <v>1</v>
       </c>
@@ -6539,7 +6702,7 @@
       </c>
       <c r="M151" s="1"/>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:16">
       <c r="A152">
         <v>-1</v>
       </c>
@@ -6582,8 +6745,11 @@
       <c r="N152" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:14">
+      <c r="P152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16">
       <c r="A153">
         <v>1</v>
       </c>
@@ -6622,7 +6788,7 @@
       </c>
       <c r="M153" s="1"/>
     </row>
-    <row r="154" spans="1:14">
+    <row r="154" spans="1:16">
       <c r="A154">
         <v>0</v>
       </c>
@@ -6661,7 +6827,7 @@
       </c>
       <c r="M154" s="1"/>
     </row>
-    <row r="155" spans="1:14">
+    <row r="155" spans="1:16">
       <c r="A155">
         <v>-1</v>
       </c>
@@ -6704,8 +6870,11 @@
       <c r="N155" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:14">
+      <c r="P155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16">
       <c r="A156">
         <v>0</v>
       </c>
@@ -6744,7 +6913,7 @@
       </c>
       <c r="M156" s="1"/>
     </row>
-    <row r="157" spans="1:14">
+    <row r="157" spans="1:16">
       <c r="A157">
         <v>1</v>
       </c>
@@ -6783,7 +6952,7 @@
       </c>
       <c r="M157" s="1"/>
     </row>
-    <row r="158" spans="1:14">
+    <row r="158" spans="1:16">
       <c r="A158">
         <v>1</v>
       </c>
@@ -6822,7 +6991,7 @@
       </c>
       <c r="M158" s="1"/>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:16">
       <c r="A159">
         <v>-1</v>
       </c>
@@ -6865,8 +7034,11 @@
       <c r="N159" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:14">
+      <c r="P159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16">
       <c r="A160">
         <v>1</v>
       </c>
@@ -6905,7 +7077,7 @@
       </c>
       <c r="M160" s="1"/>
     </row>
-    <row r="161" spans="1:14">
+    <row r="161" spans="1:16">
       <c r="A161">
         <v>1</v>
       </c>
@@ -6948,8 +7120,11 @@
       <c r="N161" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:14">
+      <c r="P161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16">
       <c r="A162">
         <v>1</v>
       </c>
@@ -6988,7 +7163,7 @@
       </c>
       <c r="M162" s="1"/>
     </row>
-    <row r="163" spans="1:14">
+    <row r="163" spans="1:16">
       <c r="A163">
         <v>1</v>
       </c>
@@ -7031,8 +7206,11 @@
       <c r="N163" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:14">
+      <c r="P163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16">
       <c r="A164">
         <v>-1</v>
       </c>
@@ -7075,8 +7253,11 @@
       <c r="N164" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:14">
+      <c r="P164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16">
       <c r="A165">
         <v>1</v>
       </c>
@@ -7115,7 +7296,7 @@
       </c>
       <c r="M165" s="1"/>
     </row>
-    <row r="166" spans="1:14">
+    <row r="166" spans="1:16">
       <c r="A166">
         <v>0</v>
       </c>
@@ -7158,8 +7339,11 @@
       <c r="N166" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:14">
+      <c r="P166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16">
       <c r="A167">
         <v>0</v>
       </c>
@@ -7198,7 +7382,7 @@
       </c>
       <c r="M167" s="1"/>
     </row>
-    <row r="168" spans="1:14">
+    <row r="168" spans="1:16">
       <c r="A168">
         <v>1</v>
       </c>
@@ -7237,7 +7421,7 @@
       </c>
       <c r="M168" s="1"/>
     </row>
-    <row r="169" spans="1:14">
+    <row r="169" spans="1:16">
       <c r="A169">
         <v>-1</v>
       </c>
@@ -7276,7 +7460,7 @@
       </c>
       <c r="M169" s="1"/>
     </row>
-    <row r="170" spans="1:14">
+    <row r="170" spans="1:16">
       <c r="A170">
         <v>0</v>
       </c>
@@ -7315,7 +7499,7 @@
       </c>
       <c r="M170" s="1"/>
     </row>
-    <row r="171" spans="1:14">
+    <row r="171" spans="1:16">
       <c r="A171">
         <v>1</v>
       </c>
@@ -7354,7 +7538,7 @@
       </c>
       <c r="M171" s="1"/>
     </row>
-    <row r="172" spans="1:14">
+    <row r="172" spans="1:16">
       <c r="A172">
         <v>1</v>
       </c>
@@ -7397,8 +7581,11 @@
       <c r="N172" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:14">
+      <c r="P172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16">
       <c r="A173">
         <v>0</v>
       </c>
@@ -7437,7 +7624,7 @@
       </c>
       <c r="M173" s="1"/>
     </row>
-    <row r="174" spans="1:14">
+    <row r="174" spans="1:16">
       <c r="A174">
         <v>-1</v>
       </c>
@@ -7476,7 +7663,7 @@
       </c>
       <c r="M174" s="1"/>
     </row>
-    <row r="175" spans="1:14">
+    <row r="175" spans="1:16">
       <c r="A175">
         <v>1</v>
       </c>
@@ -7519,8 +7706,11 @@
       <c r="N175" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:14">
+      <c r="P175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16">
       <c r="A176">
         <v>0</v>
       </c>
@@ -7563,8 +7753,11 @@
       <c r="N176" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:14">
+      <c r="P176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16">
       <c r="A177">
         <v>1</v>
       </c>
@@ -7603,7 +7796,7 @@
       </c>
       <c r="M177" s="1"/>
     </row>
-    <row r="178" spans="1:14">
+    <row r="178" spans="1:16">
       <c r="A178">
         <v>0</v>
       </c>
@@ -7642,7 +7835,7 @@
       </c>
       <c r="M178" s="1"/>
     </row>
-    <row r="179" spans="1:14">
+    <row r="179" spans="1:16">
       <c r="A179">
         <v>1</v>
       </c>
@@ -7681,7 +7874,7 @@
       </c>
       <c r="M179" s="1"/>
     </row>
-    <row r="180" spans="1:14">
+    <row r="180" spans="1:16">
       <c r="A180">
         <v>-1</v>
       </c>
@@ -7720,7 +7913,7 @@
       </c>
       <c r="M180" s="1"/>
     </row>
-    <row r="181" spans="1:14">
+    <row r="181" spans="1:16">
       <c r="A181">
         <v>-1</v>
       </c>
@@ -7759,7 +7952,7 @@
       </c>
       <c r="M181" s="1"/>
     </row>
-    <row r="182" spans="1:14">
+    <row r="182" spans="1:16">
       <c r="A182">
         <v>1</v>
       </c>
@@ -7798,7 +7991,7 @@
       </c>
       <c r="M182" s="1"/>
     </row>
-    <row r="183" spans="1:14">
+    <row r="183" spans="1:16">
       <c r="A183">
         <v>-1</v>
       </c>
@@ -7837,7 +8030,7 @@
       </c>
       <c r="M183" s="1"/>
     </row>
-    <row r="184" spans="1:14">
+    <row r="184" spans="1:16">
       <c r="A184">
         <v>1</v>
       </c>
@@ -7880,8 +8073,11 @@
       <c r="N184" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:14">
+      <c r="P184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16">
       <c r="A185">
         <v>-1</v>
       </c>
@@ -7924,8 +8120,11 @@
       <c r="N185" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:14">
+      <c r="P185" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16">
       <c r="A186">
         <v>0</v>
       </c>
@@ -7964,7 +8163,7 @@
       </c>
       <c r="M186" s="1"/>
     </row>
-    <row r="187" spans="1:14">
+    <row r="187" spans="1:16">
       <c r="A187">
         <v>0</v>
       </c>
@@ -8003,7 +8202,7 @@
       </c>
       <c r="M187" s="1"/>
     </row>
-    <row r="188" spans="1:14">
+    <row r="188" spans="1:16">
       <c r="A188">
         <v>-1</v>
       </c>
@@ -8046,8 +8245,11 @@
       <c r="N188" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:14">
+      <c r="P188" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16">
       <c r="A189">
         <v>1</v>
       </c>
@@ -8090,8 +8292,11 @@
       <c r="N189" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:14">
+      <c r="P189" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16">
       <c r="A190">
         <v>0</v>
       </c>
@@ -8130,7 +8335,7 @@
       </c>
       <c r="M190" s="1"/>
     </row>
-    <row r="191" spans="1:14">
+    <row r="191" spans="1:16">
       <c r="A191">
         <v>1</v>
       </c>
@@ -8169,7 +8374,7 @@
       </c>
       <c r="M191" s="1"/>
     </row>
-    <row r="192" spans="1:14">
+    <row r="192" spans="1:16">
       <c r="A192">
         <v>1</v>
       </c>
@@ -8212,8 +8417,11 @@
       <c r="N192" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:14">
+      <c r="P192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16">
       <c r="A193">
         <v>0</v>
       </c>
@@ -8252,7 +8460,7 @@
       </c>
       <c r="M193" s="1"/>
     </row>
-    <row r="194" spans="1:14">
+    <row r="194" spans="1:16">
       <c r="A194">
         <v>0</v>
       </c>
@@ -8291,7 +8499,7 @@
       </c>
       <c r="M194" s="1"/>
     </row>
-    <row r="195" spans="1:14">
+    <row r="195" spans="1:16">
       <c r="A195">
         <v>1</v>
       </c>
@@ -8325,7 +8533,7 @@
         <v>1</v>
       </c>
       <c r="L195" t="b">
-        <f t="shared" ref="L195:N241" si="23">(-1*(K195-2))=A195</f>
+        <f t="shared" ref="L195:L241" si="23">(-1*(K195-2))=A195</f>
         <v>1</v>
       </c>
       <c r="M195" s="1" t="b">
@@ -8334,8 +8542,11 @@
       <c r="N195" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:14">
+      <c r="P195" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16">
       <c r="A196">
         <v>1</v>
       </c>
@@ -8374,7 +8585,7 @@
       </c>
       <c r="M196" s="1"/>
     </row>
-    <row r="197" spans="1:14">
+    <row r="197" spans="1:16">
       <c r="A197">
         <v>1</v>
       </c>
@@ -8413,7 +8624,7 @@
       </c>
       <c r="M197" s="1"/>
     </row>
-    <row r="198" spans="1:14">
+    <row r="198" spans="1:16">
       <c r="A198">
         <v>-1</v>
       </c>
@@ -8452,7 +8663,7 @@
       </c>
       <c r="M198" s="1"/>
     </row>
-    <row r="199" spans="1:14">
+    <row r="199" spans="1:16">
       <c r="A199">
         <v>0</v>
       </c>
@@ -8491,7 +8702,7 @@
       </c>
       <c r="M199" s="1"/>
     </row>
-    <row r="200" spans="1:14">
+    <row r="200" spans="1:16">
       <c r="A200">
         <v>1</v>
       </c>
@@ -8534,8 +8745,11 @@
       <c r="N200" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:14">
+      <c r="P200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16">
       <c r="A201">
         <v>-1</v>
       </c>
@@ -8578,8 +8792,11 @@
       <c r="N201" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:14">
+      <c r="P201" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16">
       <c r="A202">
         <v>-1</v>
       </c>
@@ -8618,7 +8835,7 @@
       </c>
       <c r="M202" s="1"/>
     </row>
-    <row r="203" spans="1:14">
+    <row r="203" spans="1:16">
       <c r="A203">
         <v>-1</v>
       </c>
@@ -8657,7 +8874,7 @@
       </c>
       <c r="M203" s="1"/>
     </row>
-    <row r="204" spans="1:14">
+    <row r="204" spans="1:16">
       <c r="A204">
         <v>-1</v>
       </c>
@@ -8700,8 +8917,11 @@
       <c r="N204" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:14">
+      <c r="P204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16">
       <c r="A205">
         <v>-1</v>
       </c>
@@ -8740,7 +8960,7 @@
       </c>
       <c r="M205" s="1"/>
     </row>
-    <row r="206" spans="1:14">
+    <row r="206" spans="1:16">
       <c r="A206">
         <v>1</v>
       </c>
@@ -8779,7 +8999,7 @@
       </c>
       <c r="M206" s="1"/>
     </row>
-    <row r="207" spans="1:14">
+    <row r="207" spans="1:16">
       <c r="A207">
         <v>1</v>
       </c>
@@ -8822,8 +9042,11 @@
       <c r="N207" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:14">
+      <c r="P207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16">
       <c r="A208">
         <v>1</v>
       </c>
@@ -8862,7 +9085,7 @@
       </c>
       <c r="M208" s="1"/>
     </row>
-    <row r="209" spans="1:14">
+    <row r="209" spans="1:16">
       <c r="A209">
         <v>1</v>
       </c>
@@ -8905,8 +9128,11 @@
       <c r="N209" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:14">
+      <c r="P209" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16">
       <c r="A210">
         <v>0</v>
       </c>
@@ -8945,7 +9171,7 @@
       </c>
       <c r="M210" s="1"/>
     </row>
-    <row r="211" spans="1:14">
+    <row r="211" spans="1:16">
       <c r="A211">
         <v>1</v>
       </c>
@@ -8984,7 +9210,7 @@
       </c>
       <c r="M211" s="1"/>
     </row>
-    <row r="212" spans="1:14">
+    <row r="212" spans="1:16">
       <c r="A212">
         <v>1</v>
       </c>
@@ -9023,7 +9249,7 @@
       </c>
       <c r="M212" s="1"/>
     </row>
-    <row r="213" spans="1:14">
+    <row r="213" spans="1:16">
       <c r="A213">
         <v>-1</v>
       </c>
@@ -9062,7 +9288,7 @@
       </c>
       <c r="M213" s="1"/>
     </row>
-    <row r="214" spans="1:14">
+    <row r="214" spans="1:16">
       <c r="A214">
         <v>1</v>
       </c>
@@ -9105,8 +9331,11 @@
       <c r="N214" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:14">
+      <c r="P214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16">
       <c r="A215">
         <v>-1</v>
       </c>
@@ -9149,8 +9378,11 @@
       <c r="N215" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:14">
+      <c r="P215" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16">
       <c r="A216">
         <v>-1</v>
       </c>
@@ -9193,8 +9425,11 @@
       <c r="N216" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:14">
+      <c r="P216" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16">
       <c r="A217">
         <v>1</v>
       </c>
@@ -9233,7 +9468,7 @@
       </c>
       <c r="M217" s="1"/>
     </row>
-    <row r="218" spans="1:14">
+    <row r="218" spans="1:16">
       <c r="A218">
         <v>-1</v>
       </c>
@@ -9272,7 +9507,7 @@
       </c>
       <c r="M218" s="1"/>
     </row>
-    <row r="219" spans="1:14">
+    <row r="219" spans="1:16">
       <c r="A219">
         <v>-1</v>
       </c>
@@ -9315,8 +9550,11 @@
       <c r="N219" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="220" spans="1:14">
+      <c r="P219" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16">
       <c r="A220">
         <v>1</v>
       </c>
@@ -9359,8 +9597,11 @@
       <c r="N220" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:14">
+      <c r="P220" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16">
       <c r="A221">
         <v>0</v>
       </c>
@@ -9399,7 +9640,7 @@
       </c>
       <c r="M221" s="1"/>
     </row>
-    <row r="222" spans="1:14">
+    <row r="222" spans="1:16">
       <c r="A222">
         <v>1</v>
       </c>
@@ -9438,7 +9679,7 @@
       </c>
       <c r="M222" s="1"/>
     </row>
-    <row r="223" spans="1:14">
+    <row r="223" spans="1:16">
       <c r="A223">
         <v>-1</v>
       </c>
@@ -9477,7 +9718,7 @@
       </c>
       <c r="M223" s="1"/>
     </row>
-    <row r="224" spans="1:14">
+    <row r="224" spans="1:16">
       <c r="A224">
         <v>1</v>
       </c>
@@ -9520,8 +9761,11 @@
       <c r="N224" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="225" spans="1:14">
+      <c r="P224" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16">
       <c r="A225">
         <v>0</v>
       </c>
@@ -9560,7 +9804,7 @@
       </c>
       <c r="M225" s="1"/>
     </row>
-    <row r="226" spans="1:14">
+    <row r="226" spans="1:16">
       <c r="A226">
         <v>0</v>
       </c>
@@ -9603,8 +9847,11 @@
       <c r="N226" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:14">
+      <c r="P226" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16">
       <c r="A227">
         <v>0</v>
       </c>
@@ -9643,7 +9890,7 @@
       </c>
       <c r="M227" s="1"/>
     </row>
-    <row r="228" spans="1:14">
+    <row r="228" spans="1:16">
       <c r="A228">
         <v>1</v>
       </c>
@@ -9682,7 +9929,7 @@
       </c>
       <c r="M228" s="1"/>
     </row>
-    <row r="229" spans="1:14">
+    <row r="229" spans="1:16">
       <c r="A229">
         <v>0</v>
       </c>
@@ -9725,8 +9972,11 @@
       <c r="N229" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:14">
+      <c r="P229" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16">
       <c r="A230">
         <v>0</v>
       </c>
@@ -9765,7 +10015,7 @@
       </c>
       <c r="M230" s="1"/>
     </row>
-    <row r="231" spans="1:14">
+    <row r="231" spans="1:16">
       <c r="A231">
         <v>1</v>
       </c>
@@ -9808,8 +10058,11 @@
       <c r="N231" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:14">
+      <c r="P231" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16">
       <c r="A232">
         <v>0</v>
       </c>
@@ -9848,7 +10101,7 @@
       </c>
       <c r="M232" s="1"/>
     </row>
-    <row r="233" spans="1:14">
+    <row r="233" spans="1:16">
       <c r="A233">
         <v>0</v>
       </c>
@@ -9887,7 +10140,7 @@
       </c>
       <c r="M233" s="1"/>
     </row>
-    <row r="234" spans="1:14">
+    <row r="234" spans="1:16">
       <c r="A234">
         <v>1</v>
       </c>
@@ -9926,7 +10179,7 @@
       </c>
       <c r="M234" s="1"/>
     </row>
-    <row r="235" spans="1:14">
+    <row r="235" spans="1:16">
       <c r="A235">
         <v>1</v>
       </c>
@@ -9965,7 +10218,7 @@
       </c>
       <c r="M235" s="1"/>
     </row>
-    <row r="236" spans="1:14">
+    <row r="236" spans="1:16">
       <c r="A236">
         <v>-1</v>
       </c>
@@ -10004,7 +10257,7 @@
       </c>
       <c r="M236" s="1"/>
     </row>
-    <row r="237" spans="1:14">
+    <row r="237" spans="1:16">
       <c r="A237">
         <v>1</v>
       </c>
@@ -10047,8 +10300,11 @@
       <c r="N237" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:14">
+      <c r="P237" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16">
       <c r="A238">
         <v>1</v>
       </c>
@@ -10087,7 +10343,7 @@
       </c>
       <c r="M238" s="1"/>
     </row>
-    <row r="239" spans="1:14">
+    <row r="239" spans="1:16">
       <c r="A239">
         <v>1</v>
       </c>
@@ -10126,7 +10382,7 @@
       </c>
       <c r="M239" s="1"/>
     </row>
-    <row r="240" spans="1:14">
+    <row r="240" spans="1:16">
       <c r="A240">
         <v>1</v>
       </c>
@@ -10165,7 +10421,7 @@
       </c>
       <c r="M240" s="1"/>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:16">
       <c r="A241">
         <v>-1</v>
       </c>
@@ -10208,8 +10464,11 @@
       <c r="N241" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:15">
+      <c r="P241" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16">
       <c r="K242" t="s">
         <v>5</v>
       </c>
@@ -10225,8 +10484,11 @@
       <c r="O242">
         <v>84</v>
       </c>
-    </row>
-    <row r="243" spans="1:15">
+      <c r="P242">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16">
       <c r="K243" t="s">
         <v>7</v>
       </c>
@@ -10245,8 +10507,12 @@
       <c r="O243">
         <v>52</v>
       </c>
-    </row>
-    <row r="244" spans="1:15">
+      <c r="P243">
+        <f>COUNTIF(P3:P242,TRUE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16">
       <c r="K244" t="s">
         <v>6</v>
       </c>
@@ -10265,8 +10531,12 @@
       <c r="O244">
         <v>32</v>
       </c>
-    </row>
-    <row r="245" spans="1:15">
+      <c r="P244">
+        <f>P242-P243</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16">
       <c r="K245" t="s">
         <v>8</v>
       </c>
@@ -10285,6 +10555,10 @@
       <c r="O245">
         <f>(O243/O242)*100</f>
         <v>61.904761904761905</v>
+      </c>
+      <c r="P245">
+        <f>(P243/P242)*100</f>
+        <v>64.285714285714292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>